<commit_message>
Novos arquivos java script
</commit_message>
<xml_diff>
--- a/aplicativos de Mapas Mentais/Programas de Mapas Mentais.xlsx
+++ b/aplicativos de Mapas Mentais/Programas de Mapas Mentais.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\EIBNeti_PHP\aplicativos de Mapas Mentais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F485BB7C-31A2-42E9-8B81-41E94BA9E894}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E226C7-2E4A-4223-A087-7B3AEC3D33E9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7545" xr2:uid="{E65722DC-2F8F-425C-BE0F-F2E76537A596}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Planilha1!$A$1:$E$14</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
-    <t>Caracteristicas de Programas de Mapas Mentais</t>
-  </si>
-  <si>
     <t>Programas</t>
   </si>
   <si>
@@ -100,6 +94,9 @@
   </si>
   <si>
     <t>LUCID CHART</t>
+  </si>
+  <si>
+    <t>Caracteristicas de Programas de Mapas Mentais (Pesquisar e selecionar)</t>
   </si>
 </sst>
 </file>
@@ -520,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B244C658-613E-4BE3-A4E2-28FA3010C953}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,12 +526,12 @@
     <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -545,119 +542,119 @@
     </row>
     <row r="2" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -668,6 +665,6 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fechando a aula de hoje
</commit_message>
<xml_diff>
--- a/aplicativos de Mapas Mentais/Programas de Mapas Mentais.xlsx
+++ b/aplicativos de Mapas Mentais/Programas de Mapas Mentais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\EIBNeti_PHP\aplicativos de Mapas Mentais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E226C7-2E4A-4223-A087-7B3AEC3D33E9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9576B9-B875-4589-855A-B17B2569CE77}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7545" xr2:uid="{E65722DC-2F8F-425C-BE0F-F2E76537A596}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Programas</t>
   </si>
@@ -97,6 +97,24 @@
   </si>
   <si>
     <t>Caracteristicas de Programas de Mapas Mentais (Pesquisar e selecionar)</t>
+  </si>
+  <si>
+    <t>web</t>
+  </si>
+  <si>
+    <t>Somente On-line. Pagamento mensal</t>
+  </si>
+  <si>
+    <t>Pagamento mensal</t>
+  </si>
+  <si>
+    <t>Gratis e Pago</t>
+  </si>
+  <si>
+    <t>Windows - Mac</t>
+  </si>
+  <si>
+    <t>Pagamento Único em USD</t>
   </si>
 </sst>
 </file>
@@ -515,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B244C658-613E-4BE3-A4E2-28FA3010C953}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="80" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,7 +648,9 @@
       <c r="C9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -643,22 +663,38 @@
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="4"/>
+      <c r="B13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>